<commit_message>
Update data package at: 2023-09-25T08:23:40Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_classificacao_economica_despesa.xlsx
+++ b/data-raw/desc_classificacao_economica_despesa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26920"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1529042\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_56470894799A650EDC3F1BB7718E7E286798DD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D682CCE4-86C4-40F5-90AD-E135887AAA34}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_56470894799A650EDC3F1BB7718E7E286798DD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4196C53-1677-4E26-932A-56BD05B73BAB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$B$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$B$214</definedName>
     <definedName name="_GoBack" localSheetId="0">Plan1!#REF!</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="318">
   <si>
     <t>codigo</t>
   </si>
@@ -259,6 +259,9 @@
     <t>3 3 20 92</t>
   </si>
   <si>
+    <t>3 3 20 93</t>
+  </si>
+  <si>
     <t>3 3 40 41</t>
   </si>
   <si>
@@ -272,9 +275,6 @@
   </si>
   <si>
     <t>3 3 40 93</t>
-  </si>
-  <si>
-    <t>INDENIZACOES E RESTITUICOES</t>
   </si>
   <si>
     <t>3 3 41 41</t>
@@ -1316,7 +1316,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B213"/>
+  <dimension ref="A1:B214"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1651,7 +1651,7 @@
         <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1659,15 +1659,15 @@
         <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" t="s">
         <v>75</v>
-      </c>
-      <c r="B43" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1675,684 +1675,684 @@
         <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>100</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
+      </c>
+      <c r="B59" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>103</v>
-      </c>
-      <c r="B61" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B62" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B63" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B69" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B72" t="s">
-        <v>120</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B73" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B74" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B75" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B76" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B77" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B78" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B79" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B80" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B81" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B82" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B83" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B84" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B85" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B86" t="s">
-        <v>84</v>
+        <v>145</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B87" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B88" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>151</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="B89" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>153</v>
-      </c>
-      <c r="B90" t="s">
-        <v>154</v>
+        <v>151</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B91" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B92" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B93" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B94" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B95" t="s">
-        <v>88</v>
+        <v>161</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B96" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B97" t="s">
-        <v>68</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>166</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
+      </c>
+      <c r="B98" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>168</v>
-      </c>
-      <c r="B99" t="s">
-        <v>169</v>
+        <v>166</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B100" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B101" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B102" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B103" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B105" t="s">
-        <v>179</v>
+        <v>31</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B106" t="s">
-        <v>33</v>
+        <v>179</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B107" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>182</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>37</v>
+        <v>181</v>
+      </c>
+      <c r="B108" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>183</v>
-      </c>
-      <c r="B109" t="s">
-        <v>184</v>
+        <v>182</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B110" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B111" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B112" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B113" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>191</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>154</v>
+        <v>190</v>
+      </c>
+      <c r="B114" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>193</v>
-      </c>
-      <c r="B116" t="s">
-        <v>88</v>
+        <v>192</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B117" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B118" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B119" t="s">
-        <v>171</v>
+        <v>79</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B120" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B121" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B122" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B123" t="s">
-        <v>201</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B124" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B125" t="s">
-        <v>152</v>
+        <v>84</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B126" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B127" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B128" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B129" t="s">
         <v>88</v>
@@ -2360,391 +2360,391 @@
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B130" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B131" t="s">
-        <v>210</v>
+        <v>49</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B132" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B133" t="s">
-        <v>70</v>
+        <v>212</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B134" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B135" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B136" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B137" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B138" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B139" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B140" t="s">
-        <v>70</v>
+        <v>221</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B141" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B142" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B143" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B144" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B145" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B146" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B147" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B148" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B149" t="s">
-        <v>219</v>
+        <v>70</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B150" t="s">
-        <v>139</v>
+        <v>219</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B151" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B152" t="s">
-        <v>156</v>
+        <v>84</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>235</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>88</v>
+        <v>234</v>
+      </c>
+      <c r="B153" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>236</v>
-      </c>
-      <c r="B154" t="s">
-        <v>237</v>
+        <v>235</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B155" t="s">
-        <v>68</v>
+        <v>237</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B156" t="s">
-        <v>171</v>
+        <v>68</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B157" t="s">
-        <v>241</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B158" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B159" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B160" t="s">
-        <v>106</v>
+        <v>245</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B161" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B162" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B163" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B164" t="s">
-        <v>251</v>
+        <v>37</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B165" t="s">
-        <v>88</v>
+        <v>251</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B166" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B167" t="s">
-        <v>171</v>
+        <v>68</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B168" t="s">
-        <v>70</v>
+        <v>171</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B169" t="s">
-        <v>243</v>
+        <v>70</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>257</v>
-      </c>
-      <c r="B170" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B170" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>258</v>
-      </c>
-      <c r="B171" t="s">
-        <v>259</v>
+        <v>257</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>260</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>49</v>
+        <v>258</v>
+      </c>
+      <c r="B172" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>261</v>
-      </c>
-      <c r="B173" t="s">
-        <v>262</v>
+        <v>260</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B174" t="s">
-        <v>35</v>
+        <v>262</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B175" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B176" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B177" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B178" t="s">
         <v>35</v>
@@ -2752,7 +2752,7 @@
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B179" t="s">
         <v>35</v>
@@ -2760,280 +2760,287 @@
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B180" t="s">
-        <v>241</v>
+        <v>35</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B181" t="s">
-        <v>104</v>
+        <v>241</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B182" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B183" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B184" t="s">
-        <v>88</v>
+        <v>141</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B185" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B186" t="s">
-        <v>173</v>
+        <v>79</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B187" t="s">
-        <v>277</v>
+        <v>173</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B188" t="s">
-        <v>243</v>
+        <v>277</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B189" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B190" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B191" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B192" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B193" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B194" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B195" t="s">
-        <v>31</v>
+        <v>289</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B196" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B197" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B198" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B199" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B200" t="s">
-        <v>296</v>
+        <v>49</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B201" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B202" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B203" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>303</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
+      </c>
+      <c r="B204" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>33</v>
+        <v>308</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>298</v>
+        <v>37</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>37</v>
+        <v>298</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>315</v>
+        <v>37</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
+        <v>314</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
         <v>316</v>
       </c>
-      <c r="B213" s="1" t="s">
+      <c r="B214" s="1" t="s">
         <v>317</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B213" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B208">
-    <sortCondition ref="A2:A208"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B209">
+    <sortCondition ref="A2:A209"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3060,6 +3067,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c170a06b81d8b923cbfe6a63de8ee1c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="844dfdedaab7989660d9d802f918fcda" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
@@ -3308,23 +3324,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3A2F31B-1B5F-4D6E-B2EC-ACD111D3DDB3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6CA28C4-817A-47EB-86E2-CD5B69BC9DA4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902F26F7-5B6F-45AE-8405-7115E4FB3B39}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902F26F7-5B6F-45AE-8405-7115E4FB3B39}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56152C97-8754-4776-AAA1-9EB6ED60FADB}"/>
 </file>
</xml_diff>

<commit_message>
Update data package at: 2024-09-25T13:44:56Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_classificacao_economica_despesa.xlsx
+++ b/data-raw/desc_classificacao_economica_despesa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1529042\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_56470894799A650EDC3F1BB7718E7E286798DD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4196C53-1677-4E26-932A-56BD05B73BAB}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_56470894799A650EDC3F1BB7718E7E286798DD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DCB9E91-D343-4CC0-AB4A-BF1288EC1B43}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$B$214</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$B$215</definedName>
     <definedName name="_GoBack" localSheetId="0">Plan1!#REF!</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="320">
   <si>
     <t>codigo</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t>SUBVENÇÕES SOCIAIS</t>
+  </si>
+  <si>
+    <t>3 3 50 85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTRATOS DE GESTÃO </t>
   </si>
   <si>
     <t>3 3 50 92</t>
@@ -1316,9 +1322,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B215"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1763,23 +1771,23 @@
         <v>93</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1787,38 +1795,38 @@
         <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>100</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>88</v>
+      <c r="B60" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>103</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1843,31 +1851,31 @@
         <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B66" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B68" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1875,15 +1883,15 @@
         <v>114</v>
       </c>
       <c r="B69" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B70" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1891,23 +1899,23 @@
         <v>117</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B72" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B73" t="s">
-        <v>120</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1923,15 +1931,15 @@
         <v>123</v>
       </c>
       <c r="B75" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B76" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2019,15 +2027,15 @@
         <v>146</v>
       </c>
       <c r="B87" t="s">
-        <v>84</v>
+        <v>147</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B88" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2042,7 +2050,7 @@
       <c r="A90" t="s">
         <v>151</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2050,7 +2058,7 @@
       <c r="A91" t="s">
         <v>153</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="1" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2067,15 +2075,15 @@
         <v>157</v>
       </c>
       <c r="B93" t="s">
-        <v>86</v>
+        <v>158</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B94" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2091,15 +2099,15 @@
         <v>162</v>
       </c>
       <c r="B96" t="s">
-        <v>88</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B97" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2107,22 +2115,22 @@
         <v>165</v>
       </c>
       <c r="B98" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>166</v>
-      </c>
-      <c r="B99" s="1" t="s">
         <v>167</v>
+      </c>
+      <c r="B99" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>168</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="1" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2155,23 +2163,23 @@
         <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>29</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B105" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B106" t="s">
-        <v>179</v>
+        <v>31</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2179,31 +2187,31 @@
         <v>180</v>
       </c>
       <c r="B107" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B108" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>182</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>37</v>
+        <v>183</v>
+      </c>
+      <c r="B109" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>183</v>
-      </c>
-      <c r="B110" t="s">
         <v>184</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2227,28 +2235,28 @@
         <v>189</v>
       </c>
       <c r="B113" t="s">
-        <v>23</v>
+        <v>190</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B114" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>191</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>154</v>
+        <v>192</v>
+      </c>
+      <c r="B115" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>156</v>
@@ -2256,66 +2264,66 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>193</v>
-      </c>
-      <c r="B117" t="s">
-        <v>88</v>
+        <v>194</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B118" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B119" t="s">
-        <v>79</v>
+        <v>166</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B120" t="s">
-        <v>171</v>
+        <v>79</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B121" t="s">
-        <v>33</v>
+        <v>173</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B122" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B123" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B124" t="s">
-        <v>201</v>
+        <v>37</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2323,44 +2331,44 @@
         <v>202</v>
       </c>
       <c r="B125" t="s">
-        <v>84</v>
+        <v>203</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B126" t="s">
-        <v>152</v>
+        <v>84</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B127" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B128" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B129" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B130" t="s">
         <v>88</v>
@@ -2368,18 +2376,18 @@
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B131" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B132" t="s">
-        <v>210</v>
+        <v>49</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2395,47 +2403,47 @@
         <v>213</v>
       </c>
       <c r="B134" t="s">
-        <v>70</v>
+        <v>214</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B135" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B136" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B137" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B138" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B139" t="s">
-        <v>219</v>
+        <v>35</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2451,119 +2459,119 @@
         <v>222</v>
       </c>
       <c r="B141" t="s">
-        <v>70</v>
+        <v>223</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B142" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B143" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B144" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B145" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B146" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B147" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B148" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B149" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B150" t="s">
-        <v>219</v>
+        <v>70</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B151" t="s">
-        <v>139</v>
+        <v>221</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B152" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B153" t="s">
-        <v>156</v>
+        <v>84</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>235</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>88</v>
+        <v>236</v>
+      </c>
+      <c r="B154" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>236</v>
-      </c>
-      <c r="B155" t="s">
         <v>237</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2571,23 +2579,23 @@
         <v>238</v>
       </c>
       <c r="B156" t="s">
-        <v>68</v>
+        <v>239</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B157" t="s">
-        <v>171</v>
+        <v>68</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B158" t="s">
-        <v>241</v>
+        <v>173</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2611,39 +2619,39 @@
         <v>246</v>
       </c>
       <c r="B161" t="s">
-        <v>106</v>
+        <v>247</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B162" t="s">
-        <v>33</v>
+        <v>108</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B163" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B164" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B165" t="s">
-        <v>251</v>
+        <v>37</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2651,71 +2659,71 @@
         <v>252</v>
       </c>
       <c r="B166" t="s">
-        <v>88</v>
+        <v>253</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B167" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B168" t="s">
-        <v>171</v>
+        <v>68</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B169" t="s">
-        <v>70</v>
+        <v>173</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B170" t="s">
-        <v>243</v>
+        <v>70</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>257</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>243</v>
+        <v>258</v>
+      </c>
+      <c r="B171" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>258</v>
-      </c>
-      <c r="B172" t="s">
         <v>259</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
         <v>260</v>
       </c>
-      <c r="B173" s="1" t="s">
-        <v>49</v>
+      <c r="B173" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>261</v>
-      </c>
-      <c r="B174" t="s">
         <v>262</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2723,36 +2731,36 @@
         <v>263</v>
       </c>
       <c r="B175" t="s">
-        <v>35</v>
+        <v>264</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B176" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B177" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B178" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B179" t="s">
         <v>35</v>
@@ -2760,7 +2768,7 @@
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B180" t="s">
         <v>35</v>
@@ -2768,23 +2776,23 @@
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B181" t="s">
-        <v>241</v>
+        <v>35</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B182" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B183" t="s">
         <v>106</v>
@@ -2792,42 +2800,42 @@
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B184" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B185" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B186" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B187" t="s">
-        <v>173</v>
+        <v>79</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B188" t="s">
-        <v>277</v>
+        <v>175</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2835,12 +2843,12 @@
         <v>278</v>
       </c>
       <c r="B189" t="s">
-        <v>243</v>
+        <v>279</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B190" t="s">
         <v>245</v>
@@ -2848,10 +2856,10 @@
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B191" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -2891,47 +2899,47 @@
         <v>290</v>
       </c>
       <c r="B196" t="s">
-        <v>31</v>
+        <v>291</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B197" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B198" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B199" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B200" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B201" t="s">
-        <v>296</v>
+        <v>49</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2962,7 +2970,7 @@
       <c r="A205" t="s">
         <v>303</v>
       </c>
-      <c r="B205" s="1" t="s">
+      <c r="B205" t="s">
         <v>304</v>
       </c>
     </row>
@@ -2987,47 +2995,47 @@
         <v>309</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>33</v>
+        <v>310</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>298</v>
+        <v>37</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>37</v>
+        <v>300</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>315</v>
+        <v>37</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -3038,9 +3046,17 @@
         <v>317</v>
       </c>
     </row>
+    <row r="215" spans="1:2">
+      <c r="A215" t="s">
+        <v>318</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B209">
-    <sortCondition ref="A2:A209"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B210">
+    <sortCondition ref="A2:A210"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3066,15 +3082,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="18" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1b889f39a240c2e855286b20cf95d05e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="902f44b668f40cdc6ccc2fe791adf365" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
@@ -3329,14 +3336,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3A2F31B-1B5F-4D6E-B2EC-ACD111D3DDB3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902F26F7-5B6F-45AE-8405-7115E4FB3B39}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE96E9B-E27C-4DDB-AF25-5C26F198819C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE96E9B-E27C-4DDB-AF25-5C26F198819C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902F26F7-5B6F-45AE-8405-7115E4FB3B39}"/>
 </file>
</xml_diff>

<commit_message>
Update data package at: 2025-09-25T16:58:18Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_classificacao_economica_despesa.xlsx
+++ b/data-raw/desc_classificacao_economica_despesa.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28122"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1529042\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m752853\OneDrive - CAMG\General_splor\@dcppn\DCPPN 2025\PPAG e LOA 2025\PPAG\material de apoio - gerar dos volumes\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_56470894799A650EDC3F1BB7718E7E286798DD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DCB9E91-D343-4CC0-AB4A-BF1288EC1B43}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8400"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -1006,8 +1005,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1321,20 +1320,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B215"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="76.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1342,7 +1341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1350,7 +1349,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1366,7 +1365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1374,7 +1373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1390,7 +1389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1398,7 +1397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1406,7 +1405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1414,7 +1413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1422,7 +1421,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1430,7 +1429,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1438,7 +1437,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1446,7 +1445,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1454,7 +1453,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1462,7 +1461,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1478,7 +1477,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1486,7 +1485,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1494,7 +1493,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1502,7 +1501,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1526,7 +1525,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1534,7 +1533,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1542,7 +1541,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -1558,7 +1557,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1566,7 +1565,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -1574,7 +1573,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1582,7 +1581,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1590,7 +1589,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -1598,7 +1597,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>62</v>
       </c>
@@ -1606,7 +1605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -1614,7 +1613,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>64</v>
       </c>
@@ -1622,7 +1621,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -1630,7 +1629,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -1638,7 +1637,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -1662,7 +1661,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -1670,7 +1669,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -1678,7 +1677,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -1686,7 +1685,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -1694,7 +1693,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -1702,7 +1701,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>80</v>
       </c>
@@ -1710,7 +1709,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>82</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -1726,7 +1725,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -1734,7 +1733,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>87</v>
       </c>
@@ -1742,7 +1741,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>90</v>
       </c>
@@ -1758,7 +1757,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -1766,7 +1765,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>93</v>
       </c>
@@ -1774,7 +1773,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>95</v>
       </c>
@@ -1782,7 +1781,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -1798,7 +1797,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>99</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>100</v>
       </c>
@@ -1814,7 +1813,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>102</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>103</v>
       </c>
@@ -1830,7 +1829,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>105</v>
       </c>
@@ -1838,7 +1837,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>107</v>
       </c>
@@ -1846,7 +1845,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>109</v>
       </c>
@@ -1854,7 +1853,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>111</v>
       </c>
@@ -1862,7 +1861,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>112</v>
       </c>
@@ -1870,7 +1869,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>113</v>
       </c>
@@ -1878,7 +1877,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>114</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>116</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>117</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>119</v>
       </c>
@@ -1910,7 +1909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>120</v>
       </c>
@@ -1918,7 +1917,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>121</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>123</v>
       </c>
@@ -1934,7 +1933,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>125</v>
       </c>
@@ -1942,7 +1941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>126</v>
       </c>
@@ -1950,7 +1949,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>128</v>
       </c>
@@ -1958,7 +1957,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>130</v>
       </c>
@@ -1966,7 +1965,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>132</v>
       </c>
@@ -1974,7 +1973,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>134</v>
       </c>
@@ -1982,7 +1981,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>136</v>
       </c>
@@ -1990,7 +1989,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>138</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>140</v>
       </c>
@@ -2006,7 +2005,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>142</v>
       </c>
@@ -2014,7 +2013,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>144</v>
       </c>
@@ -2022,7 +2021,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>146</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>148</v>
       </c>
@@ -2038,7 +2037,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>149</v>
       </c>
@@ -2046,7 +2045,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>151</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>153</v>
       </c>
@@ -2062,7 +2061,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>155</v>
       </c>
@@ -2070,7 +2069,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>157</v>
       </c>
@@ -2078,7 +2077,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>159</v>
       </c>
@@ -2086,7 +2085,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>160</v>
       </c>
@@ -2094,7 +2093,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>162</v>
       </c>
@@ -2102,7 +2101,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>164</v>
       </c>
@@ -2110,7 +2109,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>165</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>167</v>
       </c>
@@ -2126,7 +2125,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>168</v>
       </c>
@@ -2134,7 +2133,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>170</v>
       </c>
@@ -2142,7 +2141,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>172</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>174</v>
       </c>
@@ -2158,7 +2157,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>176</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>178</v>
       </c>
@@ -2174,7 +2173,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>179</v>
       </c>
@@ -2182,7 +2181,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>180</v>
       </c>
@@ -2190,7 +2189,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>182</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>183</v>
       </c>
@@ -2206,7 +2205,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>184</v>
       </c>
@@ -2214,7 +2213,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>185</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>187</v>
       </c>
@@ -2230,7 +2229,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>189</v>
       </c>
@@ -2238,7 +2237,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>191</v>
       </c>
@@ -2246,7 +2245,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>192</v>
       </c>
@@ -2254,7 +2253,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>193</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>194</v>
       </c>
@@ -2270,7 +2269,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>195</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>196</v>
       </c>
@@ -2286,7 +2285,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>197</v>
       </c>
@@ -2294,7 +2293,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>198</v>
       </c>
@@ -2302,7 +2301,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>199</v>
       </c>
@@ -2310,7 +2309,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>200</v>
       </c>
@@ -2318,7 +2317,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>201</v>
       </c>
@@ -2326,7 +2325,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>202</v>
       </c>
@@ -2334,7 +2333,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>204</v>
       </c>
@@ -2342,7 +2341,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>205</v>
       </c>
@@ -2350,7 +2349,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>206</v>
       </c>
@@ -2358,7 +2357,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>207</v>
       </c>
@@ -2366,7 +2365,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>208</v>
       </c>
@@ -2374,7 +2373,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>209</v>
       </c>
@@ -2382,7 +2381,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>210</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>211</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>213</v>
       </c>
@@ -2406,7 +2405,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>215</v>
       </c>
@@ -2414,7 +2413,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>216</v>
       </c>
@@ -2422,7 +2421,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>217</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>218</v>
       </c>
@@ -2438,7 +2437,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>219</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>220</v>
       </c>
@@ -2454,7 +2453,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>222</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>224</v>
       </c>
@@ -2470,7 +2469,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>225</v>
       </c>
@@ -2478,7 +2477,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>226</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>227</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>228</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>229</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>230</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>231</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>232</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>233</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>234</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>235</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>236</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>237</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>238</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>240</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>241</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>242</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>244</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>246</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>248</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>249</v>
       </c>
@@ -2638,7 +2637,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>250</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>251</v>
       </c>
@@ -2654,7 +2653,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>252</v>
       </c>
@@ -2662,7 +2661,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>254</v>
       </c>
@@ -2670,7 +2669,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>255</v>
       </c>
@@ -2678,7 +2677,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>256</v>
       </c>
@@ -2686,7 +2685,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>257</v>
       </c>
@@ -2694,7 +2693,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>258</v>
       </c>
@@ -2702,7 +2701,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>259</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>260</v>
       </c>
@@ -2718,7 +2717,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>262</v>
       </c>
@@ -2726,7 +2725,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>263</v>
       </c>
@@ -2734,7 +2733,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>265</v>
       </c>
@@ -2742,7 +2741,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>266</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>267</v>
       </c>
@@ -2758,7 +2757,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>268</v>
       </c>
@@ -2766,7 +2765,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>269</v>
       </c>
@@ -2774,7 +2773,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>270</v>
       </c>
@@ -2782,7 +2781,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>271</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>272</v>
       </c>
@@ -2798,7 +2797,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>273</v>
       </c>
@@ -2806,7 +2805,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>274</v>
       </c>
@@ -2814,7 +2813,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>275</v>
       </c>
@@ -2822,7 +2821,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>276</v>
       </c>
@@ -2830,7 +2829,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>277</v>
       </c>
@@ -2838,7 +2837,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>278</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>280</v>
       </c>
@@ -2854,7 +2853,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>281</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>282</v>
       </c>
@@ -2870,7 +2869,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>284</v>
       </c>
@@ -2878,7 +2877,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>286</v>
       </c>
@@ -2886,7 +2885,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>288</v>
       </c>
@@ -2894,7 +2893,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>290</v>
       </c>
@@ -2902,7 +2901,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>292</v>
       </c>
@@ -2910,7 +2909,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>293</v>
       </c>
@@ -2918,7 +2917,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>294</v>
       </c>
@@ -2926,7 +2925,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>295</v>
       </c>
@@ -2934,7 +2933,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>296</v>
       </c>
@@ -2942,7 +2941,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>297</v>
       </c>
@@ -2950,7 +2949,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>299</v>
       </c>
@@ -2958,7 +2957,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>301</v>
       </c>
@@ -2966,7 +2965,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>303</v>
       </c>
@@ -2974,7 +2973,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>305</v>
       </c>
@@ -2982,7 +2981,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>307</v>
       </c>
@@ -2990,7 +2989,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>309</v>
       </c>
@@ -2998,7 +2997,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>311</v>
       </c>
@@ -3006,7 +3005,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>312</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>313</v>
       </c>
@@ -3022,7 +3021,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>314</v>
       </c>
@@ -3030,7 +3029,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>315</v>
       </c>
@@ -3038,7 +3037,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>316</v>
       </c>
@@ -3046,7 +3045,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>318</v>
       </c>
@@ -3055,7 +3054,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B210">
+  <sortState ref="A2:B210">
     <sortCondition ref="A2:A210"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3064,26 +3063,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="18" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1b889f39a240c2e855286b20cf95d05e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="902f44b668f40cdc6ccc2fe791adf365" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B08D58FADB61F04EBBB4F355C06EFBED" ma:contentTypeVersion="19" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7797dc5feb179b4da55a9ebddd321181">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f4338ef-addb-4c87-aefe-1895241b335f" xmlns:ns3="b91e7f20-fe0a-487d-91a9-605ac1c64acf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="90078f443198b6d5c0fd169535a443b9" ns2:_="" ns3:_="">
     <xsd:import namespace="6f4338ef-addb-4c87-aefe-1895241b335f"/>
     <xsd:import namespace="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
     <xsd:element name="properties">
@@ -3109,6 +3090,7 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3191,6 +3173,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="26" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
@@ -3336,7 +3323,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3345,14 +3332,43 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f4338ef-addb-4c87-aefe-1895241b335f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3A2F31B-1B5F-4D6E-B2EC-ACD111D3DDB3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08027DAD-E321-4F4C-ACA6-902E1CFBD038}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEE96E9B-E27C-4DDB-AF25-5C26F198819C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902F26F7-5B6F-45AE-8405-7115E4FB3B39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{902F26F7-5B6F-45AE-8405-7115E4FB3B39}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3A2F31B-1B5F-4D6E-B2EC-ACD111D3DDB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b91e7f20-fe0a-487d-91a9-605ac1c64acf"/>
+    <ds:schemaRef ds:uri="6f4338ef-addb-4c87-aefe-1895241b335f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>